<commit_message>
Resubmission of project 1
Corrected errors in analysis and report
</commit_message>
<xml_diff>
--- a/p1/P1_Data_and_Analysis.xlsx
+++ b/p1/P1_Data_and_Analysis.xlsx
@@ -1,26 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Library/Mobile Documents/com~apple~CloudDocs/education/udacity/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Histogram congruent" sheetId="11" r:id="rId2"/>
     <sheet name="Histogram incongruent" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Congruent</t>
   </si>
@@ -79,7 +71,10 @@
     <t>se(d)</t>
   </si>
   <si>
-    <t>sem</t>
+    <t>Differences</t>
+  </si>
+  <si>
+    <t>s(d)</t>
   </si>
 </sst>
 </file>
@@ -87,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -179,7 +174,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
@@ -206,7 +201,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -256,26 +251,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -330,19 +305,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -358,11 +333,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2105849440"/>
-        <c:axId val="-2105976512"/>
+        <c:axId val="38397440"/>
+        <c:axId val="38399360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2105849440"/>
+        <c:axId val="38397440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -403,26 +378,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -461,7 +416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2105976512"/>
+        <c:crossAx val="38399360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -469,7 +424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2105976512"/>
+        <c:axId val="38399360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,27 +465,8 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -561,7 +497,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2105849440"/>
+        <c:crossAx val="38397440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -645,7 +581,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -696,26 +632,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -770,19 +686,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -798,11 +714,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2112602640"/>
-        <c:axId val="-2112071664"/>
+        <c:axId val="248189312"/>
+        <c:axId val="248191232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2112602640"/>
+        <c:axId val="248189312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,26 +759,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -901,7 +797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2112071664"/>
+        <c:crossAx val="248191232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -909,7 +805,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112071664"/>
+        <c:axId val="248191232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -950,27 +846,8 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1001,7 +878,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2112602640"/>
+        <c:crossAx val="248189312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2493,7 +2370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2501,19 +2378,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:J12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2521,318 +2398,429 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>12.079000000000001</v>
       </c>
       <c r="B2" s="1">
         <v>19.277999999999999</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
+        <f>B2-A2</f>
+        <v>7.1989999999999981</v>
+      </c>
+      <c r="D2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6">
+      <c r="G2" s="6">
         <f>AVERAGE(A2:A25)</f>
         <v>14.051125000000001</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6">
+      <c r="J2" s="6">
         <f>AVERAGE(B2:B25)</f>
         <v>22.015916666666669</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="6">
-        <f>H2-E2</f>
-        <v>7.9647916666666685</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M2" s="6">
+        <f>AVERAGE(C2:C25)</f>
+        <v>7.964791666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>16.791</v>
       </c>
       <c r="B3" s="1">
         <v>18.741</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C25" si="0">B3-A3</f>
+        <v>1.9499999999999993</v>
+      </c>
+      <c r="D3">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6">
+      <c r="G3" s="6">
         <f>_xlfn.STDEV.S(A2:A25)</f>
         <v>3.559357957645187</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="6">
+      <c r="J3" s="6">
         <f>_xlfn.STDEV.S(B2:B25)</f>
         <v>4.7970571224691367</v>
       </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="6">
-        <f>SQRT(E3^2+H3^2)</f>
-        <v>5.9733396108779884</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="6">
+        <f>_xlfn.STDEV.S(C2:C25)</f>
+        <v>4.8648269103590565</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>9.5640000000000001</v>
       </c>
       <c r="B4" s="1">
         <v>21.213999999999999</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>11.649999999999999</v>
+      </c>
+      <c r="D4">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <f>COUNTA(A2:A25)</f>
         <v>24</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <f>COUNTA(B2:B25)</f>
         <v>24</v>
       </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="6">
-        <f>K3/SQRT(E4)</f>
-        <v>1.2193028422505079</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="6">
+        <f>M3/SQRT(G4)</f>
+        <v>0.9930286347783408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>8.6300000000000008</v>
       </c>
       <c r="B5" s="1">
         <v>15.686999999999999</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>7.0569999999999986</v>
+      </c>
+      <c r="D5">
         <v>40</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="7">
-        <f>E4-1</f>
+      <c r="M5" s="7">
+        <f>G4-1</f>
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>14.669</v>
       </c>
       <c r="B6" s="1">
         <v>22.803000000000001</v>
       </c>
-      <c r="J6" t="s">
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>8.1340000000000003</v>
+      </c>
+      <c r="L6" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="6">
-        <f>K2/(K3/SQRT(E4))</f>
-        <v>6.5322505539032347</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M6" s="6">
+        <f>M2/(M3/SQRT(G4))</f>
+        <v>8.0207069441099534</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>12.238</v>
       </c>
       <c r="B7" s="1">
         <v>20.878</v>
       </c>
-      <c r="J7" t="s">
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>8.64</v>
+      </c>
+      <c r="L7" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="6">
+      <c r="M7" s="6">
         <v>2.069</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>14.692</v>
       </c>
       <c r="B8" s="1">
         <v>24.571999999999999</v>
       </c>
-      <c r="J8" t="s">
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>9.879999999999999</v>
+      </c>
+      <c r="L8" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="6">
-        <f>$K$2-$K$7*$K$4</f>
-        <v>5.4420540860503674</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8" s="6">
+        <f>$M$2-$M$7*$M$4</f>
+        <v>5.9102154213102764</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8.9870000000000001</v>
       </c>
       <c r="B9" s="1">
         <v>17.393999999999998</v>
       </c>
-      <c r="J9" t="s">
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>8.4069999999999983</v>
+      </c>
+      <c r="L9" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="6">
-        <f>$K$2+$K$7*$K$4</f>
-        <v>10.48752924728297</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M9" s="6">
+        <f>$M$2+$M$7*$M$4</f>
+        <v>10.019367912023052</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9.4009999999999998</v>
       </c>
       <c r="B10" s="1">
         <v>20.762</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>11.361000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>14.48</v>
       </c>
       <c r="B11" s="1">
         <v>26.282</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>11.802</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>22.327999999999999</v>
       </c>
       <c r="B12" s="1">
         <v>24.524000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1960000000000015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>15.298</v>
       </c>
       <c r="B13" s="1">
         <v>18.643999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3459999999999983</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>15.073</v>
       </c>
       <c r="B14" s="1">
         <v>17.510000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4370000000000012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>16.928999999999998</v>
       </c>
       <c r="B15" s="1">
         <v>20.329999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4009999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>18.2</v>
       </c>
       <c r="B16" s="1">
         <v>35.255000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>17.055000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>12.13</v>
       </c>
       <c r="B17" s="1">
         <v>22.158000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>10.028</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>18.495000000000001</v>
       </c>
       <c r="B18" s="1">
         <v>25.138999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>6.6439999999999984</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>10.638999999999999</v>
       </c>
       <c r="B19" s="1">
         <v>20.428999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>9.7899999999999991</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>11.343999999999999</v>
       </c>
       <c r="B20" s="1">
         <v>17.425000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>6.0810000000000013</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>12.369</v>
       </c>
       <c r="B21" s="1">
         <v>34.287999999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>21.918999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>12.944000000000001</v>
       </c>
       <c r="B22" s="1">
         <v>23.893999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>10.949999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>14.233000000000001</v>
       </c>
       <c r="B23" s="1">
         <v>17.96</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7270000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>19.71</v>
       </c>
       <c r="B24" s="1">
         <v>22.058</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
+        <v>2.347999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>16.004000000000001</v>
       </c>
       <c r="B25" s="1">
         <v>21.157</v>
       </c>
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>5.1529999999999987</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"arial unicode ms,Bold"- Internal -</oddFooter>
+    <evenFooter>&amp;C&amp;"arial unicode ms,Bold"- Internal -</evenFooter>
+    <firstFooter>&amp;C&amp;"arial unicode ms,Bold"- Internal -</firstFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2844,9 +2832,9 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -2854,7 +2842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>10</v>
       </c>
@@ -2862,7 +2850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>20</v>
       </c>
@@ -2870,7 +2858,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>30</v>
       </c>
@@ -2878,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>40</v>
       </c>
@@ -2886,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -2899,7 +2887,13 @@
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"arial unicode ms,Bold"- Internal -</oddFooter>
+    <evenFooter>&amp;C&amp;"arial unicode ms,Bold"- Internal -</evenFooter>
+    <firstFooter>&amp;C&amp;"arial unicode ms,Bold"- Internal -</firstFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2911,9 +2905,9 @@
       <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -2921,7 +2915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>10</v>
       </c>
@@ -2929,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>20</v>
       </c>
@@ -2937,7 +2931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>30</v>
       </c>
@@ -2945,7 +2939,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>40</v>
       </c>
@@ -2953,7 +2947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -2966,6 +2960,12 @@
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"arial unicode ms,Bold"- Internal -</oddFooter>
+    <evenFooter>&amp;C&amp;"arial unicode ms,Bold"- Internal -</evenFooter>
+    <firstFooter>&amp;C&amp;"arial unicode ms,Bold"- Internal -</firstFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>